<commit_message>
avg parameters for paper
</commit_message>
<xml_diff>
--- a/LGC_Motiv_results/study1/summary_participants_infos.xlsx
+++ b/LGC_Motiv_results/study1/summary_participants_infos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clairis\Desktop\GitHub\LGC_motiv\LGC_Motiv_results\study1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8086813F-16D1-4382-9318-7FA1E888726A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FB8186-4035-4FDE-B678-4B648C8E9268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="all_subjects" sheetId="1" r:id="rId1"/>
+    <sheet name="fMRI_noSatTaskSub" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="155">
   <si>
     <t>CID066</t>
   </si>
@@ -460,6 +461,36 @@
   </si>
   <si>
     <t>06h47</t>
+  </si>
+  <si>
+    <t>avg age</t>
+  </si>
+  <si>
+    <t>std age</t>
+  </si>
+  <si>
+    <t>avg weight</t>
+  </si>
+  <si>
+    <t>std weight</t>
+  </si>
+  <si>
+    <t>avg height</t>
+  </si>
+  <si>
+    <t>std height</t>
+  </si>
+  <si>
+    <t>avg BMI</t>
+  </si>
+  <si>
+    <t>std BMI</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Height (m)</t>
   </si>
 </sst>
 </file>
@@ -627,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -718,6 +749,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1036,9 +1070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DF685-B3FD-4199-9C8B-C749A8627B53}">
   <dimension ref="A1:U128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" sqref="A1:F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7144,4 +7178,1459 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719279F6-8605-4DDB-975A-DAB8347D755B}">
+  <dimension ref="A1:O66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="7">
+        <v>72</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1.69</v>
+      </c>
+      <c r="F2" s="18">
+        <f t="shared" ref="F2:F55" si="0">D2/((E2)^2)</f>
+        <v>25.209201358495854</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(B2:B66)</f>
+        <v>29.738461538461539</v>
+      </c>
+      <c r="I2">
+        <f>STDEVA(B2:B66)</f>
+        <v>3.8821584004460501</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(D2:D66)</f>
+        <v>66.907692307692301</v>
+      </c>
+      <c r="K2">
+        <f>STDEVA(D2:D66)</f>
+        <v>11.503699237803737</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(E2:E66)</f>
+        <v>1.7146875000000001</v>
+      </c>
+      <c r="M2">
+        <f>STDEVA(E2:E66)</f>
+        <v>0.22814858940207092</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(F2:F66)</f>
+        <v>22.637472312824134</v>
+      </c>
+      <c r="O2">
+        <f>STDEVA(F2:F66)</f>
+        <v>3.9648046284251239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="7">
+        <v>31</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="7">
+        <v>65</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.79</v>
+      </c>
+      <c r="F3" s="18">
+        <f t="shared" si="0"/>
+        <v>20.286507911738084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="7">
+        <v>63</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.63</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" si="0"/>
+        <v>23.711844630960897</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="7">
+        <v>65</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.72</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>21.971335857220122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="7">
+        <v>27</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="7">
+        <v>65</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="F6" s="18">
+        <f t="shared" si="0"/>
+        <v>23.875114784205696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="7">
+        <v>67</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="0"/>
+        <v>24.609733700642796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="7">
+        <v>56</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="0"/>
+        <v>21.338210638622158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="7">
+        <v>32</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="7">
+        <v>58</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.63</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>21.829952199932254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="7">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="7">
+        <v>54</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.63</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>20.324438255109339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="7">
+        <v>31</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="7">
+        <v>85</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>26.234567901234566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="7">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="7">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1.64</v>
+      </c>
+      <c r="F12" s="18">
+        <f t="shared" si="0"/>
+        <v>21.192742415229034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>36</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="7">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" si="0"/>
+        <v>20.147971991015986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="7">
+        <v>29</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="7">
+        <v>85</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" si="0"/>
+        <v>29.411764705882355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="7">
+        <v>35</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="7">
+        <v>69</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.78</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="0"/>
+        <v>21.777553339224845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7">
+        <v>28</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="7">
+        <v>71</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1.87</v>
+      </c>
+      <c r="F16" s="18">
+        <f t="shared" si="0"/>
+        <v>20.303697560696612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="7">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="7">
+        <v>104</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
+        <v>32.098765432098766</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="7">
+        <v>39</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="7">
+        <v>66</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F18" s="18">
+        <f t="shared" si="0"/>
+        <v>21.799445105033691</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="7">
+        <v>25</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="7">
+        <v>69</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="F19" s="7">
+        <f t="shared" si="0"/>
+        <v>23.59700420642249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="7">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="7">
+        <v>60</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" si="0"/>
+        <v>20.761245674740486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="7">
+        <v>26</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="7">
+        <v>59</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1.78</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="0"/>
+        <v>18.621386188612547</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7">
+        <v>35</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="7">
+        <v>91</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1.87</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="0"/>
+        <v>26.023048986244955</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7">
+        <v>29</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="7">
+        <v>73</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1.73</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="0"/>
+        <v>24.391058839252899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="7">
+        <v>30</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="7">
+        <v>57</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1.61</v>
+      </c>
+      <c r="F24" s="7">
+        <f t="shared" si="0"/>
+        <v>21.989892365263682</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="7">
+        <v>30</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="7">
+        <v>60</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="0"/>
+        <v>21.513858510523864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="7">
+        <v>34</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="7">
+        <v>89</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1.92</v>
+      </c>
+      <c r="F26" s="18">
+        <f t="shared" si="0"/>
+        <v>24.142795138888889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7">
+        <v>31</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="7">
+        <v>68</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="0"/>
+        <v>22.204081632653061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="7">
+        <v>25</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="7">
+        <v>73</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1.81</v>
+      </c>
+      <c r="F28" s="7">
+        <f t="shared" si="0"/>
+        <v>22.282592106468055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="7">
+        <v>25</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="7">
+        <v>59</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1.57</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" si="0"/>
+        <v>23.936062314901211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="7">
+        <v>36</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="7">
+        <v>59</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1.68</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="0"/>
+        <v>20.904195011337873</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="7">
+        <v>25</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="7">
+        <v>67</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="0"/>
+        <v>21.877551020408163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="7">
+        <v>25</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="7">
+        <v>59</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1.72</v>
+      </c>
+      <c r="F32" s="7">
+        <f t="shared" si="0"/>
+        <v>19.943212547322879</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="7">
+        <v>30</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="7">
+        <v>64</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1.64</v>
+      </c>
+      <c r="F33" s="18">
+        <f t="shared" si="0"/>
+        <v>23.795359904818564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="7">
+        <v>25</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="7">
+        <v>78</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" si="0"/>
+        <v>22.790357925493058</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="7">
+        <v>35</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="7">
+        <v>101</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1.88</v>
+      </c>
+      <c r="F35" s="18">
+        <f t="shared" si="0"/>
+        <v>28.576278859212316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="7">
+        <v>34</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="7">
+        <v>67</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1.78</v>
+      </c>
+      <c r="F36" s="18">
+        <f t="shared" si="0"/>
+        <v>21.146319909102385</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="7">
+        <v>26</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="7">
+        <v>64</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="F37" s="18">
+        <f t="shared" si="0"/>
+        <v>21.887076365377382</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="7">
+        <v>26</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="7">
+        <v>69</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="0"/>
+        <v>21.296296296296294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="7">
+        <v>33</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="7">
+        <v>71</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="0"/>
+        <v>22.662708672475979</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="7">
+        <v>28</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="7">
+        <v>83</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F40" s="18">
+        <f t="shared" si="0"/>
+        <v>27.414453692693883</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="7">
+        <v>27</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="7">
+        <v>63</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1.68</v>
+      </c>
+      <c r="F41" s="18">
+        <f t="shared" si="0"/>
+        <v>22.321428571428577</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="7">
+        <v>26</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="7">
+        <v>58</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1.63</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="0"/>
+        <v>21.829952199932254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="7">
+        <v>36</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="7">
+        <v>63</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1.66</v>
+      </c>
+      <c r="F43" s="18">
+        <f t="shared" si="0"/>
+        <v>22.862534475250399</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="7">
+        <v>39</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="7">
+        <v>80</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1.83</v>
+      </c>
+      <c r="F44" s="18">
+        <f t="shared" si="0"/>
+        <v>23.888440980620498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="7">
+        <v>32</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="7">
+        <v>62</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="F45" s="18">
+        <f t="shared" si="0"/>
+        <v>19.1358024691358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="7">
+        <v>31</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="7">
+        <v>54</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="F46" s="18">
+        <f t="shared" si="0"/>
+        <v>20.576131687242793</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="7">
+        <v>28</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="7">
+        <v>53</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1.68</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="0"/>
+        <v>18.778344671201818</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="7">
+        <v>30</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="7">
+        <v>62</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F48" s="7">
+        <f t="shared" si="0"/>
+        <v>20.478266613819528</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7">
+        <v>30</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="7">
+        <v>70</v>
+      </c>
+      <c r="E49" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F49" s="18">
+        <f t="shared" si="0"/>
+        <v>23.120623596247853</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="7">
+        <v>25</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="7">
+        <v>56</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1.63</v>
+      </c>
+      <c r="F50" s="18">
+        <f t="shared" si="0"/>
+        <v>21.077195227520797</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="7">
+        <v>28</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="7">
+        <v>51</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" si="0"/>
+        <v>19.433013260173752</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="7">
+        <v>27</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="7">
+        <v>54</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1.53</v>
+      </c>
+      <c r="F52" s="18">
+        <f t="shared" si="0"/>
+        <v>23.068050749711649</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="7">
+        <v>27</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="7">
+        <v>51</v>
+      </c>
+      <c r="E53" s="7">
+        <v>1.72</v>
+      </c>
+      <c r="F53" s="7">
+        <f t="shared" si="0"/>
+        <v>17.239048134126556</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="7">
+        <v>36</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="7">
+        <v>65</v>
+      </c>
+      <c r="E54" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="F54" s="18">
+        <f t="shared" si="0"/>
+        <v>25.390624999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="7">
+        <v>31</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="7">
+        <v>50</v>
+      </c>
+      <c r="E55" s="7">
+        <v>1.68</v>
+      </c>
+      <c r="F55" s="18">
+        <f t="shared" si="0"/>
+        <v>17.715419501133791</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="7">
+        <v>25</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="7">
+        <v>56</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1.56</v>
+      </c>
+      <c r="F56" s="7">
+        <f t="shared" ref="F56:F61" si="1">D56/((E56)^2)</f>
+        <v>23.011176857330703</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="7">
+        <v>29</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="7">
+        <v>76</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" si="1"/>
+        <v>23.456790123456788</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="7">
+        <v>30</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="7">
+        <v>65</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" si="1"/>
+        <v>21.224489795918366</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="7">
+        <v>26</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="7">
+        <v>71</v>
+      </c>
+      <c r="E59" s="7">
+        <v>1.73</v>
+      </c>
+      <c r="F59" s="18">
+        <f t="shared" si="1"/>
+        <v>23.722810651876106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="7">
+        <v>35</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="7">
+        <v>51</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1.64</v>
+      </c>
+      <c r="F60" s="18">
+        <f t="shared" si="1"/>
+        <v>18.961927424152293</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="7">
+        <v>27</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="7">
+        <v>67</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1.72</v>
+      </c>
+      <c r="F61" s="18">
+        <f t="shared" si="1"/>
+        <v>22.647376960519203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="7">
+        <v>29</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="7">
+        <v>72</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="7">
+        <v>27</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="7">
+        <v>80</v>
+      </c>
+      <c r="E63" s="7">
+        <v>1.79</v>
+      </c>
+      <c r="F63" s="7">
+        <f>D63/((E63)^2)</f>
+        <v>24.968009737523797</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="7">
+        <v>28</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="7">
+        <v>63</v>
+      </c>
+      <c r="E64" s="7">
+        <v>1.73</v>
+      </c>
+      <c r="F64" s="7">
+        <f>D64/((E64)^2)</f>
+        <v>21.04981790236894</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="7">
+        <v>29</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="7">
+        <v>72</v>
+      </c>
+      <c r="E65" s="7">
+        <v>1.69</v>
+      </c>
+      <c r="F65" s="7">
+        <f>D65/((E65)^2)</f>
+        <v>25.209201358495854</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="7">
+        <v>29</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="7">
+        <v>81</v>
+      </c>
+      <c r="E66" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="F66" s="18">
+        <f>D66/((E66)^2)</f>
+        <v>29.752066115702483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding missing money info
</commit_message>
<xml_diff>
--- a/LGC_Motiv_results/study1/summary_participants_infos.xlsx
+++ b/LGC_Motiv_results/study1/summary_participants_infos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clairis\Desktop\GitHub\LGC_motiv\LGC_Motiv_results\study1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FB8186-4035-4FDE-B678-4B648C8E9268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A602C9E-67A4-4ABC-9E01-3BC6A26F0052}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
   </bookViews>
   <sheets>
     <sheet name="all_subjects" sheetId="1" r:id="rId1"/>
     <sheet name="fMRI_noSatTaskSub" sheetId="2" r:id="rId2"/>
+    <sheet name="payment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="157">
   <si>
     <t>CID066</t>
   </si>
@@ -491,6 +492,24 @@
   </si>
   <si>
     <t>Height (m)</t>
+  </si>
+  <si>
+    <t>ID participant</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Somme remportée </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(CHF)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -500,7 +519,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,8 +550,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +585,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -753,6 +796,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7184,7 +7246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719279F6-8605-4DDB-975A-DAB8347D755B}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -8633,4 +8695,838 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E44DB92-EB4E-43C9-BB01-4A269A4106C9}">
+  <dimension ref="A1:D125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="22.7109375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>230</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(B2:B76)</f>
+        <v>201.44</v>
+      </c>
+      <c r="D2">
+        <f>STDEVA(B2:B76)</f>
+        <v>19.74036884564628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="38">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="39">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75" s="3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="4"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="4"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="4"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="4"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="4"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="4"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="4"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="4"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="4"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="4"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="4"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="4"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="4"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="4"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="4"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="4"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="4"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="4"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="4"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="4"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="B111" s="4"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="4"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="4"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="4"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="4"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="4"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="4"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="4"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="4"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="4"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="4"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="4"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update with subjects included
</commit_message>
<xml_diff>
--- a/LGC_Motiv_results/study1/summary_participants_infos.xlsx
+++ b/LGC_Motiv_results/study1/summary_participants_infos.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clairis\Desktop\GitHub\LGC_motiv\LGC_Motiv_results\study1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EE134-9FC9-4F07-9AD1-8984FEDBDD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{541D1A55-30F0-4F1A-8375-8EEDA9D8EC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{973ACBFE-62E1-4B63-85AE-C8E6F8B95C54}"/>
   </bookViews>
   <sheets>
     <sheet name="all_subjects" sheetId="1" r:id="rId1"/>
     <sheet name="all_subjects_no_pilots" sheetId="4" r:id="rId2"/>
     <sheet name="fMRI_noSatTaskSub" sheetId="2" r:id="rId3"/>
-    <sheet name="payment" sheetId="3" r:id="rId4"/>
+    <sheet name="fMRI_noSatTaskSub_bis" sheetId="5" r:id="rId4"/>
+    <sheet name="payment" sheetId="3" r:id="rId5"/>
+    <sheet name="payment_fMRI_noSatTaskSub_bis" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="188">
   <si>
     <t>CID066</t>
   </si>
@@ -642,6 +645,9 @@
   <si>
     <t>Apprentissage</t>
   </si>
+  <si>
+    <t>Note: same as fMRI_noSatTaskSub but also removing 2 subjects with too big head (CID054 and CID090)</t>
+  </si>
 </sst>
 </file>
 
@@ -859,7 +865,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -988,17 +994,9 @@
     <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutre" xfId="1" builtinId="28"/>
@@ -1317,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DF685-B3FD-4199-9C8B-C749A8627B53}">
   <dimension ref="A1:AB128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U3" sqref="U3"/>
     </sheetView>
@@ -1335,7 +1333,7 @@
     <col min="22" max="22" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="345.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>101</v>
       </c>
@@ -1486,29 +1484,29 @@
       <c r="U2" s="29">
         <v>7</v>
       </c>
-      <c r="V2" s="46" t="s">
+      <c r="V2" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="W2" s="47" t="s">
+      <c r="W2" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="X2" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="49" t="s">
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="AA2" s="48">
+      <c r="AA2">
         <v>8</v>
       </c>
-      <c r="AB2" s="48">
+      <c r="AB2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>27</v>
       </c>
@@ -1573,29 +1571,29 @@
       <c r="U3" s="29">
         <v>7</v>
       </c>
-      <c r="V3" s="46" t="s">
+      <c r="V3" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="W3" s="47" t="s">
+      <c r="W3" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="X3" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="48" t="s">
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
         <v>157</v>
       </c>
-      <c r="AA3" s="48">
+      <c r="AA3">
         <v>8</v>
       </c>
-      <c r="AB3" s="48">
+      <c r="AB3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>36</v>
       </c>
@@ -1660,29 +1658,29 @@
       <c r="U4" s="29">
         <v>4</v>
       </c>
-      <c r="V4" s="46" t="s">
+      <c r="V4" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="W4" s="47" t="s">
+      <c r="W4" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="X4" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="46" t="s">
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AA4" s="48">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <v>3</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>70</v>
       </c>
@@ -1747,25 +1745,25 @@
       <c r="U5" s="29">
         <v>4</v>
       </c>
-      <c r="V5" s="46" t="s">
+      <c r="V5" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="W5" s="47" t="s">
+      <c r="W5" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="X5" s="48">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="48" t="s">
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>160</v>
       </c>
-      <c r="AA5" s="48">
+      <c r="AA5">
         <v>12</v>
       </c>
-      <c r="AB5" s="48">
+      <c r="AB5">
         <v>8</v>
       </c>
     </row>
@@ -1834,29 +1832,29 @@
       <c r="U6" s="29">
         <v>7</v>
       </c>
-      <c r="V6" s="46" t="s">
+      <c r="V6" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="W6" s="47" t="s">
+      <c r="W6" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="X6" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="48">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="46" t="s">
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AA6" s="48">
+      <c r="AA6">
         <v>8</v>
       </c>
-      <c r="AB6" s="48">
+      <c r="AB6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
@@ -1921,25 +1919,25 @@
       <c r="U7" s="29">
         <v>5</v>
       </c>
-      <c r="V7" s="46" t="s">
+      <c r="V7" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="W7" s="47" t="s">
+      <c r="W7" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="X7" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="48" t="s">
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="s">
         <v>157</v>
       </c>
-      <c r="AA7" s="48">
+      <c r="AA7">
         <v>8</v>
       </c>
-      <c r="AB7" s="48">
+      <c r="AB7">
         <v>7</v>
       </c>
     </row>
@@ -2008,25 +2006,25 @@
       <c r="U8" s="29">
         <v>7</v>
       </c>
-      <c r="V8" s="46" t="s">
+      <c r="V8" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="W8" s="47" t="s">
+      <c r="W8" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="X8" s="48">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="48" t="s">
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
         <v>163</v>
       </c>
-      <c r="AA8" s="48">
-        <v>3</v>
-      </c>
-      <c r="AB8" s="48">
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
         <v>3</v>
       </c>
     </row>
@@ -2095,25 +2093,25 @@
       <c r="U9" s="29">
         <v>9</v>
       </c>
-      <c r="V9" s="48" t="s">
+      <c r="V9" t="s">
         <v>175</v>
       </c>
-      <c r="W9" s="50">
+      <c r="W9" s="40">
         <v>120000</v>
       </c>
-      <c r="X9" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="48" t="s">
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="s">
         <v>157</v>
       </c>
-      <c r="AA9" s="48">
+      <c r="AA9">
         <v>8</v>
       </c>
-      <c r="AB9" s="48">
+      <c r="AB9">
         <v>7</v>
       </c>
     </row>
@@ -2182,29 +2180,29 @@
       <c r="U10" s="29">
         <v>8</v>
       </c>
-      <c r="V10" s="48" t="s">
+      <c r="V10" t="s">
         <v>167</v>
       </c>
-      <c r="W10" s="50">
+      <c r="W10" s="40">
         <v>60000</v>
       </c>
-      <c r="X10" s="48">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="48" t="s">
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="s">
         <v>157</v>
       </c>
-      <c r="AA10" s="48">
+      <c r="AA10">
         <v>8</v>
       </c>
-      <c r="AB10" s="48">
+      <c r="AB10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
@@ -2269,25 +2267,25 @@
       <c r="U11" s="29">
         <v>5</v>
       </c>
-      <c r="V11" s="46" t="s">
+      <c r="V11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="W11" s="47" t="s">
+      <c r="W11" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="X11" s="48">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="48">
-        <v>3</v>
-      </c>
-      <c r="Z11" s="46" t="s">
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AA11" s="48">
-        <v>3</v>
-      </c>
-      <c r="AB11" s="48">
+      <c r="AA11">
+        <v>3</v>
+      </c>
+      <c r="AB11">
         <v>3</v>
       </c>
     </row>
@@ -2356,29 +2354,29 @@
       <c r="U12" s="29">
         <v>4</v>
       </c>
-      <c r="V12" s="46" t="s">
+      <c r="V12" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="W12" s="47" t="s">
+      <c r="W12" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="X12" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="48">
-        <v>4</v>
-      </c>
-      <c r="Z12" s="46" t="s">
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AA12" s="48">
+      <c r="AA12">
         <v>8</v>
       </c>
-      <c r="AB12" s="48">
+      <c r="AB12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
@@ -2437,25 +2435,25 @@
       <c r="U13" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="V13" s="46" t="s">
+      <c r="V13" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="W13" s="47" t="s">
+      <c r="W13" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="X13" s="48">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="48" t="s">
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="s">
         <v>157</v>
       </c>
-      <c r="AA13" s="48">
+      <c r="AA13">
         <v>8</v>
       </c>
-      <c r="AB13" s="48">
+      <c r="AB13">
         <v>7</v>
       </c>
     </row>
@@ -2524,25 +2522,25 @@
       <c r="U14" s="29">
         <v>5</v>
       </c>
-      <c r="V14" s="46" t="s">
+      <c r="V14" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="W14" s="47" t="s">
+      <c r="W14" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="X14" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="48">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="46" t="s">
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AA14" s="48">
+      <c r="AA14">
         <v>8</v>
       </c>
-      <c r="AB14" s="48">
+      <c r="AB14">
         <v>7</v>
       </c>
     </row>
@@ -2611,29 +2609,29 @@
       <c r="U15" s="29">
         <v>7</v>
       </c>
-      <c r="V15" s="48" t="s">
+      <c r="V15" t="s">
         <v>165</v>
       </c>
-      <c r="W15" s="50">
+      <c r="W15" s="40">
         <v>40000</v>
       </c>
-      <c r="X15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="48" t="s">
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
         <v>160</v>
       </c>
-      <c r="AA15" s="48">
+      <c r="AA15">
         <v>12</v>
       </c>
-      <c r="AB15" s="48">
+      <c r="AB15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>18</v>
       </c>
@@ -2698,29 +2696,29 @@
       <c r="U16" s="29">
         <v>4</v>
       </c>
-      <c r="V16" s="46" t="s">
+      <c r="V16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="W16" s="47" t="s">
+      <c r="W16" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="X16" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="48" t="s">
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
         <v>157</v>
       </c>
-      <c r="AA16" s="48">
+      <c r="AA16">
         <v>8</v>
       </c>
-      <c r="AB16" s="48">
+      <c r="AB16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
@@ -2785,25 +2783,25 @@
       <c r="U17" s="29">
         <v>5</v>
       </c>
-      <c r="V17" s="46" t="s">
+      <c r="V17" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="W17" s="47" t="s">
+      <c r="W17" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="X17" s="48">
-        <v>2</v>
-      </c>
-      <c r="Y17" s="48">
-        <v>2</v>
-      </c>
-      <c r="Z17" s="49" t="s">
+      <c r="X17">
+        <v>2</v>
+      </c>
+      <c r="Y17">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="AA17" s="48">
-        <v>3</v>
-      </c>
-      <c r="AB17" s="48">
+      <c r="AA17">
+        <v>3</v>
+      </c>
+      <c r="AB17">
         <v>3</v>
       </c>
     </row>
@@ -2872,29 +2870,29 @@
       <c r="U18" s="29">
         <v>1</v>
       </c>
-      <c r="V18" s="46" t="s">
+      <c r="V18" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="W18" s="47" t="s">
+      <c r="W18" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="X18" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="48" t="s">
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
         <v>163</v>
       </c>
-      <c r="AA18" s="48">
-        <v>3</v>
-      </c>
-      <c r="AB18" s="48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="AA18">
+        <v>3</v>
+      </c>
+      <c r="AB18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>69</v>
       </c>
@@ -2959,25 +2957,25 @@
       <c r="U19" s="29">
         <v>5</v>
       </c>
-      <c r="V19" s="46" t="s">
+      <c r="V19" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="W19" s="47" t="s">
+      <c r="W19" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="X19" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="48" t="s">
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
         <v>157</v>
       </c>
-      <c r="AA19" s="48">
+      <c r="AA19">
         <v>8</v>
       </c>
-      <c r="AB19" s="48">
+      <c r="AB19">
         <v>7</v>
       </c>
     </row>
@@ -3046,25 +3044,25 @@
       <c r="U20" s="29">
         <v>5</v>
       </c>
-      <c r="V20" s="46" t="s">
+      <c r="V20" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="W20" s="47" t="s">
+      <c r="W20" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="X20" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="46" t="s">
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="AA20" s="48">
+      <c r="AA20">
         <v>6</v>
       </c>
-      <c r="AB20" s="48">
+      <c r="AB20">
         <v>5</v>
       </c>
     </row>
@@ -3385,7 +3383,7 @@
       <c r="Y24">
         <v>0</v>
       </c>
-      <c r="Z24" s="49" t="s">
+      <c r="Z24" s="46" t="s">
         <v>157</v>
       </c>
       <c r="AA24">
@@ -3395,7 +3393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>66</v>
       </c>
@@ -3743,7 +3741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>12</v>
       </c>
@@ -3830,7 +3828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>29</v>
       </c>
@@ -4178,7 +4176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>15</v>
       </c>
@@ -4516,7 +4514,7 @@
       <c r="Y37">
         <v>4</v>
       </c>
-      <c r="Z37" s="49" t="s">
+      <c r="Z37" s="46" t="s">
         <v>157</v>
       </c>
       <c r="AA37">
@@ -4874,7 +4872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>22</v>
       </c>
@@ -4961,7 +4959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>20</v>
       </c>
@@ -5048,7 +5046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>26</v>
       </c>
@@ -5307,7 +5305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>17</v>
       </c>
@@ -5394,7 +5392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>7</v>
       </c>
@@ -5481,7 +5479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>65</v>
       </c>
@@ -5568,7 +5566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>6</v>
       </c>
@@ -5655,7 +5653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>16</v>
       </c>
@@ -5808,7 +5806,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>41</v>
       </c>
@@ -6156,7 +6154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>71</v>
       </c>
@@ -6243,7 +6241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>3</v>
       </c>
@@ -6330,7 +6328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>43</v>
       </c>
@@ -6591,7 +6589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>9</v>
       </c>
@@ -7024,7 +7022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>68</v>
       </c>
@@ -7198,7 +7196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>10</v>
       </c>
@@ -7372,7 +7370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>8</v>
       </c>
@@ -7459,7 +7457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>63</v>
       </c>
@@ -7698,7 +7696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>72</v>
       </c>
@@ -7785,7 +7783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>5</v>
       </c>
@@ -7872,7 +7870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>64</v>
       </c>
@@ -8046,7 +8044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>33</v>
       </c>
@@ -14276,8 +14274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719279F6-8605-4DDB-975A-DAB8347D755B}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15728,11 +15726,1427 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101FFF18-9D57-4178-82CB-6CB45647161A}">
+  <dimension ref="A1:O64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:A64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="6">
+        <v>72</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1.69</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" ref="F2:F59" si="0">D2/((E2)^2)</f>
+        <v>25.209201358495854</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(B2:B64)</f>
+        <v>29.698412698412699</v>
+      </c>
+      <c r="I2">
+        <f>STDEVA(B2:B64)</f>
+        <v>3.8714626753060419</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(D2:D64)</f>
+        <v>66.365079365079367</v>
+      </c>
+      <c r="K2">
+        <f>STDEVA(D2:D64)</f>
+        <v>10.842422041195702</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(E2:E64)</f>
+        <v>1.7119354838709679</v>
+      </c>
+      <c r="M2">
+        <f>STDEVA(E2:E64)</f>
+        <v>0.23045436986497389</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(F2:F64)</f>
+        <v>22.541525358080854</v>
+      </c>
+      <c r="O2">
+        <f>STDEVA(F2:F64)</f>
+        <v>3.9466251425805008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6">
+        <v>31</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6">
+        <v>65</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.79</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>20.286507911738084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="6">
+        <v>63</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="0"/>
+        <v>23.711844630960897</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.72</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
+        <v>21.971335857220122</v>
+      </c>
+      <c r="H5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="6">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="6">
+        <v>65</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.65</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>23.875114784205696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="6">
+        <v>67</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.65</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="0"/>
+        <v>24.609733700642796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="6">
+        <v>56</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.62</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="0"/>
+        <v>21.338210638622158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="6">
+        <v>32</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="6">
+        <v>58</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="0"/>
+        <v>21.829952199932254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="6">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="6">
+        <v>54</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>20.324438255109339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="6">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="6">
+        <v>85</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>26.234567901234566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="6">
+        <v>57</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="0"/>
+        <v>21.192742415229034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>36</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="6">
+        <v>61</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="0"/>
+        <v>20.147971991015986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="6">
+        <v>29</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="6">
+        <v>85</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="0"/>
+        <v>29.411764705882355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="6">
+        <v>35</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="6">
+        <v>69</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>21.777553339224845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="6">
+        <v>71</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.87</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="0"/>
+        <v>20.303697560696612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="6">
+        <v>39</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="6">
+        <v>104</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>32.098765432098766</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="6">
+        <v>39</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="6">
+        <v>66</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" si="0"/>
+        <v>21.799445105033691</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="6">
+        <v>25</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="6">
+        <v>69</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.71</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>23.59700420642249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>28</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="6">
+        <v>60</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="0"/>
+        <v>20.761245674740486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="6">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="6">
+        <v>59</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="F21" s="17">
+        <f t="shared" si="0"/>
+        <v>18.621386188612547</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="6">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="6">
+        <v>91</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.87</v>
+      </c>
+      <c r="F22" s="17">
+        <f t="shared" si="0"/>
+        <v>26.023048986244955</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="6">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6">
+        <v>73</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="0"/>
+        <v>24.391058839252899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="6">
+        <v>30</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="6">
+        <v>57</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>21.989892365263682</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6">
+        <v>30</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="6">
+        <v>60</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="F25" s="17">
+        <f t="shared" si="0"/>
+        <v>21.513858510523864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="6">
+        <v>34</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="6">
+        <v>89</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1.92</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="0"/>
+        <v>24.142795138888889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="6">
+        <v>31</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="6">
+        <v>68</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="0"/>
+        <v>22.204081632653061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="6">
+        <v>25</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="6">
+        <v>73</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1.81</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="0"/>
+        <v>22.282592106468055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="6">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="6">
+        <v>59</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1.57</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="0"/>
+        <v>23.936062314901211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="6">
+        <v>36</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="6">
+        <v>59</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="F30" s="17">
+        <f t="shared" si="0"/>
+        <v>20.904195011337873</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="6">
+        <v>25</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="6">
+        <v>67</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="F31" s="17">
+        <f t="shared" si="0"/>
+        <v>21.877551020408163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="6">
+        <v>25</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="6">
+        <v>59</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1.72</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="0"/>
+        <v>19.943212547322879</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6">
+        <v>30</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="6">
+        <v>64</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="0"/>
+        <v>23.795359904818564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="6">
+        <v>25</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="6">
+        <v>78</v>
+      </c>
+      <c r="E34" s="6">
+        <v>1.85</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="0"/>
+        <v>22.790357925493058</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="6">
+        <v>34</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="6">
+        <v>67</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="F35" s="17">
+        <f t="shared" si="0"/>
+        <v>21.146319909102385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="6">
+        <v>26</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="6">
+        <v>64</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1.71</v>
+      </c>
+      <c r="F36" s="17">
+        <f t="shared" si="0"/>
+        <v>21.887076365377382</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="6">
+        <v>26</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="6">
+        <v>69</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F37" s="6">
+        <f t="shared" si="0"/>
+        <v>21.296296296296294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="6">
+        <v>33</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="6">
+        <v>71</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1.77</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" si="0"/>
+        <v>22.662708672475979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="6">
+        <v>28</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="6">
+        <v>83</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F39" s="17">
+        <f t="shared" si="0"/>
+        <v>27.414453692693883</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="6">
+        <v>27</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="6">
+        <v>63</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="F40" s="17">
+        <f t="shared" si="0"/>
+        <v>22.321428571428577</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="6">
+        <v>26</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="6">
+        <v>58</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="F41" s="6">
+        <f t="shared" si="0"/>
+        <v>21.829952199932254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="6">
+        <v>36</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="6">
+        <v>63</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1.66</v>
+      </c>
+      <c r="F42" s="17">
+        <f t="shared" si="0"/>
+        <v>22.862534475250399</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="6">
+        <v>39</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="6">
+        <v>80</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1.83</v>
+      </c>
+      <c r="F43" s="17">
+        <f t="shared" si="0"/>
+        <v>23.888440980620498</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="6">
+        <v>32</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="6">
+        <v>62</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F44" s="17">
+        <f t="shared" si="0"/>
+        <v>19.1358024691358</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="6">
+        <v>31</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6">
+        <v>54</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1.62</v>
+      </c>
+      <c r="F45" s="17">
+        <f t="shared" si="0"/>
+        <v>20.576131687242793</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="6">
+        <v>28</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="6">
+        <v>53</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="0"/>
+        <v>18.778344671201818</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="6">
+        <v>30</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="6">
+        <v>62</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F47" s="6">
+        <f t="shared" si="0"/>
+        <v>20.478266613819528</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="6">
+        <v>30</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="6">
+        <v>70</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F48" s="17">
+        <f t="shared" si="0"/>
+        <v>23.120623596247853</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="6">
+        <v>25</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="6">
+        <v>56</v>
+      </c>
+      <c r="E49" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="F49" s="17">
+        <f t="shared" si="0"/>
+        <v>21.077195227520797</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="6">
+        <v>28</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="6">
+        <v>51</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1.62</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" si="0"/>
+        <v>19.433013260173752</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="6">
+        <v>27</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="6">
+        <v>54</v>
+      </c>
+      <c r="E51" s="6">
+        <v>1.53</v>
+      </c>
+      <c r="F51" s="17">
+        <f t="shared" si="0"/>
+        <v>23.068050749711649</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="6">
+        <v>27</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="6">
+        <v>51</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1.72</v>
+      </c>
+      <c r="F52" s="6">
+        <f t="shared" si="0"/>
+        <v>17.239048134126556</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="6">
+        <v>36</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="6">
+        <v>65</v>
+      </c>
+      <c r="E53" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F53" s="17">
+        <f t="shared" si="0"/>
+        <v>25.390624999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="6">
+        <v>31</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="6">
+        <v>50</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="F54" s="17">
+        <f t="shared" si="0"/>
+        <v>17.715419501133791</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="6">
+        <v>25</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="6">
+        <v>56</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1.56</v>
+      </c>
+      <c r="F55" s="6">
+        <f t="shared" si="0"/>
+        <v>23.011176857330703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="6">
+        <v>29</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="6">
+        <v>76</v>
+      </c>
+      <c r="E56" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F56" s="6">
+        <f t="shared" si="0"/>
+        <v>23.456790123456788</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="6">
+        <v>30</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="6">
+        <v>65</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="F57" s="6">
+        <f t="shared" si="0"/>
+        <v>21.224489795918366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="6">
+        <v>26</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="6">
+        <v>71</v>
+      </c>
+      <c r="E58" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="F58" s="17">
+        <f t="shared" si="0"/>
+        <v>23.722810651876106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="6">
+        <v>35</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="6">
+        <v>51</v>
+      </c>
+      <c r="E59" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="F59" s="17">
+        <f t="shared" si="0"/>
+        <v>18.961927424152293</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="6">
+        <v>29</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="6">
+        <v>72</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="6">
+        <v>27</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="6">
+        <v>80</v>
+      </c>
+      <c r="E61" s="6">
+        <v>1.79</v>
+      </c>
+      <c r="F61" s="6">
+        <f>D61/((E61)^2)</f>
+        <v>24.968009737523797</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="6">
+        <v>28</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="6">
+        <v>63</v>
+      </c>
+      <c r="E62" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="F62" s="6">
+        <f>D62/((E62)^2)</f>
+        <v>21.04981790236894</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="6">
+        <v>29</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="6">
+        <v>72</v>
+      </c>
+      <c r="E63" s="6">
+        <v>1.69</v>
+      </c>
+      <c r="F63" s="6">
+        <f>D63/((E63)^2)</f>
+        <v>25.209201358495854</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="6">
+        <v>29</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="6">
+        <v>81</v>
+      </c>
+      <c r="E64" s="6">
+        <v>1.65</v>
+      </c>
+      <c r="F64" s="17">
+        <f>D64/((E64)^2)</f>
+        <v>29.752066115702483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E44DB92-EB4E-43C9-BB01-4A269A4106C9}">
   <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B76"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16559,4 +17973,745 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68048CB8-3465-4E0F-BDE0-95FEE42D95C4}">
+  <dimension ref="A1:D113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="37">
+        <v>234</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(B2:B64)</f>
+        <v>203.17460317460316</v>
+      </c>
+      <c r="D2">
+        <f>STDEVA(B2:B64)</f>
+        <v>15.574523948132651</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="38">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="4"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="4"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="4"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="4"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="4"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="4"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="4"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="4"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="4"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="4"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="4"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="4"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="4"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="4"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="4"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="4"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="4"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="4"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="4"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="4"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="4"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="4"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="4"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="4"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="4"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="4"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="4"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="4"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="4"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="B111" s="4"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B114">
+    <sortCondition ref="A2:A114"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>